<commit_message>
update p_post, replace to p_ra instead.
</commit_message>
<xml_diff>
--- a/cicat/cvss-example/SCENARIO-new-fake.xlsx
+++ b/cicat/cvss-example/SCENARIO-new-fake.xlsx
@@ -6247,7 +6247,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6282,7 +6282,7 @@
         <v>86</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.22</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6291,7 +6291,7 @@
         <v>83</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6300,7 +6300,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>